<commit_message>
Update to US commit ecc67274 on 6/5/24
</commit_message>
<xml_diff>
--- a/InputData/elec/BDTPTUMCF/Boolean Does This Plant Type Use Maximum Capacity Factor.xlsx
+++ b/InputData/elec/BDTPTUMCF/Boolean Does This Plant Type Use Maximum Capacity Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\BDTPTUMCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BDTPTUMCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ED9A98-533A-401F-8B39-EF71FBE64D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DCE9AD-342C-4F1D-9344-9510E0382F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="1695" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -893,7 +893,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="3"/>
     </row>

</xml_diff>